<commit_message>
removed old regulator circuits
a better chip (tested) has been found rt7272a
</commit_message>
<xml_diff>
--- a/First order list.xlsx
+++ b/First order list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{389D787C-4146-4585-A43E-9E44B5CCB696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42E22559-4109-49C0-8139-E846DAF36289}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{389D787C-4146-4585-A43E-9E44B5CCB696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F92AD28C-B12D-44F3-BA77-6A2100192A3A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20250" windowHeight="11520" xr2:uid="{D63B4B4D-3BD8-437A-B6D9-F138B7A04AC4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D63B4B4D-3BD8-437A-B6D9-F138B7A04AC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Component</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>24V 10A PSU</t>
+  </si>
+  <si>
+    <t>https://nl.aliexpress.com/item/32917996858.html?gatewayAdapt=glo2nld</t>
+  </si>
+  <si>
+    <t>stepper motor protector</t>
   </si>
 </sst>
 </file>
@@ -466,7 +472,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,7 +585,15 @@
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C9" s="1"/>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>

</xml_diff>